<commit_message>
se actualiza el formato "Matriz de Pruebas"
</commit_message>
<xml_diff>
--- a/02-Pruebas/Spooler-Distribucion-Matriz_Pruebas.xlsx
+++ b/02-Pruebas/Spooler-Distribucion-Matriz_Pruebas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion-spooler\02-Pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\02-Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD584E7-084B-4502-AA29-87DA1C5A74BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2457B2E1-3F72-49DD-AEE8-109E2BD2273A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$E$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$F$117</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -80,7 +80,7 @@
     ID_CRON con el que se puede probar el proceso una vez que se terminó de Migrar.</t>
       </text>
     </comment>
-    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
+    <comment ref="F1" authorId="4" shapeId="0" xr:uid="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -88,7 +88,7 @@
     Observaciones o comentarios que se consideren importantes al migrar un módulo.</t>
       </text>
     </comment>
-    <comment ref="F1" authorId="5" shapeId="0" xr:uid="{BF8F3FBD-6206-4492-AAB1-C20E746C84BC}">
+    <comment ref="G1" authorId="5" shapeId="0" xr:uid="{BF8F3FBD-6206-4492-AAB1-C20E746C84BC}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -96,7 +96,7 @@
     Listar los LayOut’s utilizados para realizar pruebas (txt, xls, etc).</t>
       </text>
     </comment>
-    <comment ref="G1" authorId="6" shapeId="0" xr:uid="{B2A12130-6F6A-4049-B368-A74E2C9EAC5B}">
+    <comment ref="H1" authorId="6" shapeId="0" xr:uid="{B2A12130-6F6A-4049-B368-A74E2C9EAC5B}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="222">
   <si>
     <t>Nombre Reporte</t>
   </si>
@@ -772,13 +772,16 @@
   </si>
   <si>
     <t>ARCHIVOS DE ENTRADA</t>
+  </si>
+  <si>
+    <t>FECHA DE PRUEBA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -804,12 +807,6 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -920,6 +917,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -931,12 +934,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1241,13 +1238,13 @@
   <threadedComment ref="D1" dT="2025-04-23T23:38:33.71" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{38372124-5616-401A-B40A-476DE7B44D8B}">
     <text>ID_CRON con el que se puede probar el proceso una vez que se terminó de Migrar.</text>
   </threadedComment>
-  <threadedComment ref="E1" dT="2025-04-23T23:38:58.34" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
+  <threadedComment ref="F1" dT="2025-04-23T23:38:58.34" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
     <text>Observaciones o comentarios que se consideren importantes al migrar un módulo.</text>
   </threadedComment>
-  <threadedComment ref="F1" dT="2025-06-10T15:27:46.66" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{BF8F3FBD-6206-4492-AAB1-C20E746C84BC}">
+  <threadedComment ref="G1" dT="2025-06-10T15:27:46.66" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{BF8F3FBD-6206-4492-AAB1-C20E746C84BC}">
     <text>Listar los LayOut’s utilizados para realizar pruebas (txt, xls, etc).</text>
   </threadedComment>
-  <threadedComment ref="G1" dT="2025-06-04T15:56:50.77" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{B2A12130-6F6A-4049-B368-A74E2C9EAC5B}">
+  <threadedComment ref="H1" dT="2025-06-04T15:56:50.77" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{B2A12130-6F6A-4049-B368-A74E2C9EAC5B}">
     <text>Incluir el listado de Archivos (txt, xls, doc, mail, etc…) que se generaron al realizar las pruebas.</text>
   </threadedComment>
 </ThreadedComments>
@@ -1255,11 +1252,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
-  <dimension ref="A1:G117"/>
+  <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,44 +1264,48 @@
     <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="80.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="80.5703125" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="80.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="80.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="10" t="s">
         <v>219</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="10" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>206</v>
       </c>
@@ -1313,11 +1314,12 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>132</v>
       </c>
@@ -1326,11 +1328,12 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>208</v>
       </c>
@@ -1339,11 +1342,12 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>210</v>
       </c>
@@ -1352,11 +1356,12 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>83</v>
       </c>
@@ -1365,11 +1370,12 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>200</v>
       </c>
@@ -1378,11 +1384,12 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>201</v>
       </c>
@@ -1391,11 +1398,12 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>172</v>
       </c>
@@ -1404,11 +1412,12 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>154</v>
       </c>
@@ -1417,11 +1426,12 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>152</v>
       </c>
@@ -1430,11 +1440,12 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="2"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>212</v>
       </c>
@@ -1443,11 +1454,12 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>151</v>
       </c>
@@ -1456,11 +1468,12 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>194</v>
       </c>
@@ -1469,11 +1482,12 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>203</v>
       </c>
@@ -1482,11 +1496,12 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>204</v>
       </c>
@@ -1495,11 +1510,12 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>202</v>
       </c>
@@ -1508,11 +1524,12 @@
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3"/>
       <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>183</v>
       </c>
@@ -1521,11 +1538,12 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="1"/>
       <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>182</v>
       </c>
@@ -1534,11 +1552,12 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="3"/>
+      <c r="E20" s="4"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>215</v>
       </c>
@@ -1550,8 +1569,9 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>214</v>
       </c>
@@ -1560,11 +1580,12 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="3"/>
       <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>143</v>
       </c>
@@ -1573,11 +1594,12 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="1"/>
       <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>180</v>
       </c>
@@ -1586,11 +1608,12 @@
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="3"/>
       <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>146</v>
       </c>
@@ -1599,11 +1622,12 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="1"/>
       <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>160</v>
       </c>
@@ -1612,11 +1636,12 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="3"/>
       <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>164</v>
       </c>
@@ -1625,11 +1650,12 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>159</v>
       </c>
@@ -1641,8 +1667,9 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>86</v>
       </c>
@@ -1651,11 +1678,12 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="1"/>
       <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>169</v>
       </c>
@@ -1664,11 +1692,12 @@
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="3"/>
       <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -1677,11 +1706,12 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="1"/>
       <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -1690,11 +1720,12 @@
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="1"/>
       <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>52</v>
       </c>
@@ -1703,11 +1734,12 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="3"/>
       <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>20</v>
       </c>
@@ -1716,11 +1748,12 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="1"/>
       <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>23</v>
       </c>
@@ -1729,11 +1762,12 @@
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="3"/>
       <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>24</v>
       </c>
@@ -1742,11 +1776,12 @@
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="1"/>
       <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>21</v>
       </c>
@@ -1755,11 +1790,12 @@
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="3"/>
       <c r="G37" s="4"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>141</v>
       </c>
@@ -1768,11 +1804,12 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="1"/>
       <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>17</v>
       </c>
@@ -1781,11 +1818,12 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="3"/>
       <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>22</v>
       </c>
@@ -1794,11 +1832,12 @@
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="1"/>
       <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>18</v>
       </c>
@@ -1807,11 +1846,12 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="3"/>
       <c r="G41" s="4"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>19</v>
       </c>
@@ -1820,11 +1860,12 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="4"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="3"/>
       <c r="G42" s="4"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>188</v>
       </c>
@@ -1833,11 +1874,12 @@
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="4"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="3"/>
       <c r="G43" s="4"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>189</v>
       </c>
@@ -1846,11 +1888,12 @@
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="1"/>
       <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>153</v>
       </c>
@@ -1859,11 +1902,12 @@
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="4"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="3"/>
       <c r="G45" s="4"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>196</v>
       </c>
@@ -1872,11 +1916,12 @@
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="2"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="1"/>
       <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>126</v>
       </c>
@@ -1885,11 +1930,12 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="4"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="3"/>
       <c r="G47" s="4"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>31</v>
       </c>
@@ -1898,11 +1944,12 @@
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="2"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="1"/>
       <c r="G48" s="2"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>59</v>
       </c>
@@ -1911,11 +1958,12 @@
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="1"/>
       <c r="G49" s="2"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>61</v>
       </c>
@@ -1924,11 +1972,12 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="3"/>
       <c r="G50" s="4"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>157</v>
       </c>
@@ -1937,11 +1986,12 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="4"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="3"/>
       <c r="G51" s="4"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>168</v>
       </c>
@@ -1950,11 +2000,12 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="4"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="3"/>
       <c r="G52" s="4"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>186</v>
       </c>
@@ -1963,11 +2014,12 @@
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="1"/>
       <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>199</v>
       </c>
@@ -1976,11 +2028,12 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="4"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="3"/>
       <c r="G54" s="4"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>111</v>
       </c>
@@ -1989,11 +2042,12 @@
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="1"/>
       <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>140</v>
       </c>
@@ -2002,11 +2056,12 @@
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="4"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="3"/>
       <c r="G56" s="4"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>12</v>
       </c>
@@ -2015,11 +2070,12 @@
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="4"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="3"/>
       <c r="G57" s="4"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>15</v>
       </c>
@@ -2028,11 +2084,12 @@
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="2"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="1"/>
       <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>16</v>
       </c>
@@ -2041,11 +2098,12 @@
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="4"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="3"/>
       <c r="G59" s="4"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59" s="4"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>170</v>
       </c>
@@ -2054,11 +2112,12 @@
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="1"/>
       <c r="G60" s="2"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>144</v>
       </c>
@@ -2067,11 +2126,12 @@
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="2"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="1"/>
       <c r="G61" s="2"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>192</v>
       </c>
@@ -2080,11 +2140,12 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="4"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="3"/>
       <c r="G62" s="4"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>191</v>
       </c>
@@ -2093,11 +2154,12 @@
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="1"/>
       <c r="G63" s="2"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>96</v>
       </c>
@@ -2106,11 +2168,12 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="4"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="3"/>
       <c r="G64" s="4"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>187</v>
       </c>
@@ -2119,11 +2182,12 @@
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="4"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="3"/>
       <c r="G65" s="4"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65" s="4"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>150</v>
       </c>
@@ -2132,11 +2196,12 @@
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="2"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="1"/>
       <c r="G66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>123</v>
       </c>
@@ -2145,11 +2210,12 @@
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="4"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="3"/>
       <c r="G67" s="4"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67" s="4"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>174</v>
       </c>
@@ -2158,11 +2224,12 @@
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="2"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="1"/>
       <c r="G68" s="2"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>10</v>
       </c>
@@ -2171,11 +2238,12 @@
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="4"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="3"/>
       <c r="G69" s="4"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69" s="4"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>33</v>
       </c>
@@ -2184,11 +2252,12 @@
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="2"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="1"/>
       <c r="G70" s="2"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>178</v>
       </c>
@@ -2197,11 +2266,12 @@
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="4"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="3"/>
       <c r="G71" s="4"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71" s="4"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>128</v>
       </c>
@@ -2210,11 +2280,12 @@
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="2"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="1"/>
       <c r="G72" s="2"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>142</v>
       </c>
@@ -2223,11 +2294,12 @@
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="4"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="3"/>
       <c r="G73" s="4"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73" s="4"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>147</v>
       </c>
@@ -2236,11 +2308,12 @@
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="2"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="1"/>
       <c r="G74" s="2"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>148</v>
       </c>
@@ -2249,11 +2322,12 @@
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="4"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="3"/>
       <c r="G75" s="4"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75" s="4"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>145</v>
       </c>
@@ -2262,11 +2336,12 @@
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="1"/>
       <c r="G76" s="2"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76" s="2"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>98</v>
       </c>
@@ -2275,11 +2350,12 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="4"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="3"/>
       <c r="G77" s="4"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77" s="4"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>45</v>
       </c>
@@ -2288,11 +2364,12 @@
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="4"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="3"/>
       <c r="G78" s="4"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78" s="4"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>176</v>
       </c>
@@ -2301,11 +2378,12 @@
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="2"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="1"/>
       <c r="G79" s="2"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79" s="2"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>72</v>
       </c>
@@ -2314,11 +2392,12 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="4"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="3"/>
       <c r="G80" s="4"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80" s="4"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>197</v>
       </c>
@@ -2327,11 +2406,12 @@
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="2"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="1"/>
       <c r="G81" s="2"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H81" s="2"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>181</v>
       </c>
@@ -2340,11 +2420,12 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="4"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="3"/>
       <c r="G82" s="4"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H82" s="4"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>103</v>
       </c>
@@ -2353,11 +2434,12 @@
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="2"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="1"/>
       <c r="G83" s="2"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83" s="2"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>158</v>
       </c>
@@ -2366,11 +2448,12 @@
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="4"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="3"/>
       <c r="G84" s="4"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84" s="4"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>155</v>
       </c>
@@ -2379,11 +2462,12 @@
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="4"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="3"/>
       <c r="G85" s="4"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85" s="4"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>171</v>
       </c>
@@ -2392,11 +2476,12 @@
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="4"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="3"/>
       <c r="G86" s="4"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86" s="4"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>14</v>
       </c>
@@ -2405,11 +2490,12 @@
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="4"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="3"/>
       <c r="G87" s="4"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H87" s="4"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>165</v>
       </c>
@@ -2418,11 +2504,12 @@
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="2"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="1"/>
       <c r="G88" s="2"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88" s="2"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>167</v>
       </c>
@@ -2431,11 +2518,12 @@
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="4"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="3"/>
       <c r="G89" s="4"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89" s="4"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>8</v>
       </c>
@@ -2444,11 +2532,12 @@
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="2"/>
-      <c r="E90" s="1"/>
-      <c r="F90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="1"/>
       <c r="G90" s="2"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90" s="2"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>27</v>
       </c>
@@ -2457,11 +2546,12 @@
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="4"/>
-      <c r="E91" s="3"/>
-      <c r="F91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="3"/>
       <c r="G91" s="4"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H91" s="4"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>162</v>
       </c>
@@ -2470,11 +2560,12 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="4"/>
-      <c r="E92" s="3"/>
-      <c r="F92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="3"/>
       <c r="G92" s="4"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92" s="4"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>179</v>
       </c>
@@ -2483,11 +2574,12 @@
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="2"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="1"/>
       <c r="G93" s="2"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93" s="2"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>163</v>
       </c>
@@ -2496,11 +2588,12 @@
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="4"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="3"/>
       <c r="G94" s="4"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94" s="4"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>166</v>
       </c>
@@ -2509,11 +2602,12 @@
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="2"/>
-      <c r="E95" s="1"/>
-      <c r="F95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="1"/>
       <c r="G95" s="2"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95" s="2"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>193</v>
       </c>
@@ -2522,11 +2616,12 @@
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="4"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="3"/>
       <c r="G96" s="4"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H96" s="4"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>29</v>
       </c>
@@ -2535,11 +2630,12 @@
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="2"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="1"/>
       <c r="G97" s="2"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H97" s="2"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>177</v>
       </c>
@@ -2548,11 +2644,12 @@
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="4"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="3"/>
       <c r="G98" s="4"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98" s="4"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>173</v>
       </c>
@@ -2561,11 +2658,12 @@
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="2"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="1"/>
       <c r="G99" s="2"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H99" s="2"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>195</v>
       </c>
@@ -2574,11 +2672,12 @@
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="4"/>
-      <c r="E100" s="3"/>
-      <c r="F100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="3"/>
       <c r="G100" s="4"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100" s="4"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>185</v>
       </c>
@@ -2587,11 +2686,12 @@
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="2"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="1"/>
       <c r="G101" s="2"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H101" s="2"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>149</v>
       </c>
@@ -2600,11 +2700,12 @@
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="4"/>
-      <c r="E102" s="3"/>
-      <c r="F102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="3"/>
       <c r="G102" s="4"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H102" s="4"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>156</v>
       </c>
@@ -2613,11 +2714,12 @@
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="2"/>
-      <c r="E103" s="1"/>
-      <c r="F103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="1"/>
       <c r="G103" s="2"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H103" s="2"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>175</v>
       </c>
@@ -2626,11 +2728,12 @@
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="2"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="1"/>
       <c r="G104" s="2"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H104" s="2"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>109</v>
       </c>
@@ -2639,11 +2742,12 @@
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="4"/>
-      <c r="E105" s="3"/>
-      <c r="F105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="3"/>
       <c r="G105" s="4"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H105" s="4"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>25</v>
       </c>
@@ -2652,11 +2756,12 @@
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="2"/>
-      <c r="E106" s="1"/>
-      <c r="F106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="1"/>
       <c r="G106" s="2"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H106" s="2"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>190</v>
       </c>
@@ -2665,11 +2770,12 @@
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="2"/>
-      <c r="E107" s="1"/>
-      <c r="F107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="1"/>
       <c r="G107" s="2"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H107" s="2"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>57</v>
       </c>
@@ -2678,11 +2784,12 @@
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="4"/>
-      <c r="E108" s="3"/>
-      <c r="F108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="3"/>
       <c r="G108" s="4"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H108" s="4"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>6</v>
       </c>
@@ -2691,11 +2798,12 @@
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="2"/>
-      <c r="E109" s="1"/>
-      <c r="F109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="1"/>
       <c r="G109" s="2"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H109" s="2"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>198</v>
       </c>
@@ -2704,11 +2812,12 @@
       </c>
       <c r="C110" s="3"/>
       <c r="D110" s="4"/>
-      <c r="E110" s="3"/>
-      <c r="F110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="3"/>
       <c r="G110" s="4"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H110" s="4"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>161</v>
       </c>
@@ -2717,11 +2826,12 @@
       </c>
       <c r="C111" s="3"/>
       <c r="D111" s="4"/>
-      <c r="E111" s="3"/>
-      <c r="F111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="3"/>
       <c r="G111" s="4"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H111" s="4"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>50</v>
       </c>
@@ -2730,11 +2840,12 @@
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="2"/>
-      <c r="E112" s="1"/>
-      <c r="F112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="1"/>
       <c r="G112" s="2"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H112" s="2"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>134</v>
       </c>
@@ -2743,11 +2854,12 @@
       </c>
       <c r="C113" s="3"/>
       <c r="D113" s="4"/>
-      <c r="E113" s="3"/>
-      <c r="F113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="3"/>
       <c r="G113" s="4"/>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H113" s="4"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>54</v>
       </c>
@@ -2756,11 +2868,12 @@
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="2"/>
-      <c r="E114" s="1"/>
-      <c r="F114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="1"/>
       <c r="G114" s="2"/>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H114" s="2"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>184</v>
       </c>
@@ -2769,11 +2882,12 @@
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="2"/>
-      <c r="E115" s="1"/>
-      <c r="F115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="1"/>
       <c r="G115" s="2"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H115" s="2"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>118</v>
       </c>
@@ -2782,11 +2896,12 @@
       </c>
       <c r="C116" s="1"/>
       <c r="D116" s="2"/>
-      <c r="E116" s="1"/>
-      <c r="F116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="1"/>
       <c r="G116" s="2"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H116" s="2"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>120</v>
       </c>
@@ -2795,23 +2910,25 @@
       </c>
       <c r="C117" s="7"/>
       <c r="D117" s="8"/>
-      <c r="E117" s="7"/>
-      <c r="F117" s="8"/>
+      <c r="E117" s="8"/>
+      <c r="F117" s="7"/>
       <c r="G117" s="8"/>
+      <c r="H117" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E117" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E117">
+  <autoFilter ref="A2:F117" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F117">
     <sortCondition ref="A3:A117"/>
   </sortState>
-  <mergeCells count="7">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="E1:E2"/>
+  <mergeCells count="8">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se actualiza versión de comunicación a BD's y se sube primera versión estable del aplicativo, lista para ejecutar en el servidor de desarrollo.
</commit_message>
<xml_diff>
--- a/02-Pruebas/Spooler-Distribucion-Matriz_Pruebas.xlsx
+++ b/02-Pruebas/Spooler-Distribucion-Matriz_Pruebas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\02-Pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion-spooler\02-Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2457B2E1-3F72-49DD-AEE8-109E2BD2273A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A078F5A8-8A30-4453-9B44-5AA16957E730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
     Nombre de quién migró el módulo.</t>
       </text>
     </comment>
-    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{38372124-5616-401A-B40A-476DE7B44D8B}">
+    <comment ref="E1" authorId="3" shapeId="0" xr:uid="{38372124-5616-401A-B40A-476DE7B44D8B}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1235,7 +1235,7 @@
   <threadedComment ref="C1" dT="2025-06-10T15:28:01.40" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{71F5E753-58EC-4771-AF81-BADB944F6AB9}">
     <text>Nombre de quién migró el módulo.</text>
   </threadedComment>
-  <threadedComment ref="D1" dT="2025-04-23T23:38:33.71" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{38372124-5616-401A-B40A-476DE7B44D8B}">
+  <threadedComment ref="E1" dT="2025-04-23T23:38:33.71" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{38372124-5616-401A-B40A-476DE7B44D8B}">
     <text>ID_CRON con el que se puede probar el proceso una vez que se terminó de Migrar.</text>
   </threadedComment>
   <threadedComment ref="F1" dT="2025-04-23T23:38:58.34" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
@@ -1263,8 +1263,8 @@
   <cols>
     <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="5" width="17.7109375" customWidth="1"/>
+    <col min="3" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="80.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="80.5703125" customWidth="1"/>
   </cols>
@@ -1279,11 +1279,11 @@
       <c r="C1" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>219</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>221</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>138</v>
@@ -1299,7 +1299,7 @@
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="15"/>
-      <c r="D2" s="11"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
       <c r="G2" s="11"/>
@@ -1313,7 +1313,7 @@
         <v>207</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="4"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1327,7 +1327,7 @@
         <v>133</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="2"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1341,7 +1341,7 @@
         <v>209</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="4"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -1355,7 +1355,7 @@
         <v>211</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="2"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1369,7 +1369,7 @@
         <v>84</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="4"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1383,7 +1383,7 @@
         <v>130</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="1"/>
       <c r="E8" s="2"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1397,7 +1397,7 @@
         <v>131</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -1411,7 +1411,7 @@
         <v>81</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10" s="1"/>
       <c r="G10" s="2"/>
@@ -1425,7 +1425,7 @@
         <v>49</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="4"/>
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
@@ -1439,7 +1439,7 @@
         <v>47</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="1"/>
       <c r="E12" s="2"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1453,7 +1453,7 @@
         <v>213</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1467,7 +1467,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="9"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="9"/>
       <c r="F14" s="6"/>
       <c r="G14" s="9"/>
@@ -1481,7 +1481,7 @@
         <v>114</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="2"/>
       <c r="F15" s="1"/>
       <c r="G15" s="2"/>
@@ -1495,7 +1495,7 @@
         <v>137</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="3"/>
       <c r="E16" s="4"/>
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
@@ -1509,7 +1509,7 @@
         <v>205</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="1"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1"/>
       <c r="G17" s="2"/>
@@ -1523,7 +1523,7 @@
         <v>136</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="3"/>
       <c r="E18" s="4"/>
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
@@ -1537,7 +1537,7 @@
         <v>95</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="2"/>
       <c r="F19" s="1"/>
       <c r="G19" s="2"/>
@@ -1551,7 +1551,7 @@
         <v>94</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="4"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1579,7 +1579,7 @@
         <v>217</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="4"/>
       <c r="F22" s="3"/>
       <c r="G22" s="4"/>
@@ -1593,7 +1593,7 @@
         <v>36</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
+      <c r="D23" s="1"/>
       <c r="E23" s="2"/>
       <c r="F23" s="1"/>
       <c r="G23" s="2"/>
@@ -1607,7 +1607,7 @@
         <v>92</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="4"/>
       <c r="F24" s="3"/>
       <c r="G24" s="4"/>
@@ -1621,7 +1621,7 @@
         <v>39</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="1"/>
       <c r="E25" s="2"/>
       <c r="F25" s="1"/>
       <c r="G25" s="2"/>
@@ -1635,7 +1635,7 @@
         <v>67</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
+      <c r="D26" s="3"/>
       <c r="E26" s="4"/>
       <c r="F26" s="3"/>
       <c r="G26" s="4"/>
@@ -1649,7 +1649,7 @@
         <v>71</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
+      <c r="D27" s="1"/>
       <c r="E27" s="2"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1677,7 +1677,7 @@
         <v>87</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
+      <c r="D29" s="1"/>
       <c r="E29" s="2"/>
       <c r="F29" s="1"/>
       <c r="G29" s="2"/>
@@ -1691,7 +1691,7 @@
         <v>78</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="3"/>
       <c r="E30" s="4"/>
       <c r="F30" s="3"/>
       <c r="G30" s="4"/>
@@ -1705,7 +1705,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
+      <c r="D31" s="1"/>
       <c r="E31" s="2"/>
       <c r="F31" s="1"/>
       <c r="G31" s="2"/>
@@ -1719,7 +1719,7 @@
         <v>5</v>
       </c>
       <c r="C32" s="1"/>
-      <c r="D32" s="2"/>
+      <c r="D32" s="1"/>
       <c r="E32" s="2"/>
       <c r="F32" s="1"/>
       <c r="G32" s="2"/>
@@ -1733,7 +1733,7 @@
         <v>53</v>
       </c>
       <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
+      <c r="D33" s="3"/>
       <c r="E33" s="4"/>
       <c r="F33" s="3"/>
       <c r="G33" s="4"/>
@@ -1747,7 +1747,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="1"/>
-      <c r="D34" s="2"/>
+      <c r="D34" s="1"/>
       <c r="E34" s="2"/>
       <c r="F34" s="1"/>
       <c r="G34" s="2"/>
@@ -1761,7 +1761,7 @@
         <v>7</v>
       </c>
       <c r="C35" s="3"/>
-      <c r="D35" s="4"/>
+      <c r="D35" s="3"/>
       <c r="E35" s="4"/>
       <c r="F35" s="3"/>
       <c r="G35" s="4"/>
@@ -1775,7 +1775,7 @@
         <v>7</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="2"/>
+      <c r="D36" s="1"/>
       <c r="E36" s="2"/>
       <c r="F36" s="1"/>
       <c r="G36" s="2"/>
@@ -1789,7 +1789,7 @@
         <v>7</v>
       </c>
       <c r="C37" s="3"/>
-      <c r="D37" s="4"/>
+      <c r="D37" s="3"/>
       <c r="E37" s="4"/>
       <c r="F37" s="3"/>
       <c r="G37" s="4"/>
@@ -1803,7 +1803,7 @@
         <v>7</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="2"/>
+      <c r="D38" s="1"/>
       <c r="E38" s="2"/>
       <c r="F38" s="1"/>
       <c r="G38" s="2"/>
@@ -1817,7 +1817,7 @@
         <v>7</v>
       </c>
       <c r="C39" s="3"/>
-      <c r="D39" s="4"/>
+      <c r="D39" s="3"/>
       <c r="E39" s="4"/>
       <c r="F39" s="3"/>
       <c r="G39" s="4"/>
@@ -1831,7 +1831,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="1"/>
-      <c r="D40" s="2"/>
+      <c r="D40" s="1"/>
       <c r="E40" s="2"/>
       <c r="F40" s="1"/>
       <c r="G40" s="2"/>
@@ -1845,7 +1845,7 @@
         <v>7</v>
       </c>
       <c r="C41" s="3"/>
-      <c r="D41" s="4"/>
+      <c r="D41" s="3"/>
       <c r="E41" s="4"/>
       <c r="F41" s="3"/>
       <c r="G41" s="4"/>
@@ -1859,7 +1859,7 @@
         <v>7</v>
       </c>
       <c r="C42" s="3"/>
-      <c r="D42" s="4"/>
+      <c r="D42" s="3"/>
       <c r="E42" s="4"/>
       <c r="F42" s="3"/>
       <c r="G42" s="4"/>
@@ -1873,7 +1873,7 @@
         <v>106</v>
       </c>
       <c r="C43" s="3"/>
-      <c r="D43" s="4"/>
+      <c r="D43" s="3"/>
       <c r="E43" s="4"/>
       <c r="F43" s="3"/>
       <c r="G43" s="4"/>
@@ -1887,7 +1887,7 @@
         <v>107</v>
       </c>
       <c r="C44" s="1"/>
-      <c r="D44" s="2"/>
+      <c r="D44" s="1"/>
       <c r="E44" s="2"/>
       <c r="F44" s="1"/>
       <c r="G44" s="2"/>
@@ -1901,7 +1901,7 @@
         <v>48</v>
       </c>
       <c r="C45" s="3"/>
-      <c r="D45" s="4"/>
+      <c r="D45" s="3"/>
       <c r="E45" s="4"/>
       <c r="F45" s="3"/>
       <c r="G45" s="4"/>
@@ -1915,7 +1915,7 @@
         <v>116</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="2"/>
+      <c r="D46" s="1"/>
       <c r="E46" s="2"/>
       <c r="F46" s="1"/>
       <c r="G46" s="2"/>
@@ -1929,7 +1929,7 @@
         <v>127</v>
       </c>
       <c r="C47" s="3"/>
-      <c r="D47" s="4"/>
+      <c r="D47" s="3"/>
       <c r="E47" s="4"/>
       <c r="F47" s="3"/>
       <c r="G47" s="4"/>
@@ -1943,7 +1943,7 @@
         <v>32</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="2"/>
+      <c r="D48" s="1"/>
       <c r="E48" s="2"/>
       <c r="F48" s="1"/>
       <c r="G48" s="2"/>
@@ -1957,7 +1957,7 @@
         <v>60</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="2"/>
+      <c r="D49" s="1"/>
       <c r="E49" s="2"/>
       <c r="F49" s="1"/>
       <c r="G49" s="2"/>
@@ -1971,7 +1971,7 @@
         <v>62</v>
       </c>
       <c r="C50" s="3"/>
-      <c r="D50" s="4"/>
+      <c r="D50" s="3"/>
       <c r="E50" s="4"/>
       <c r="F50" s="3"/>
       <c r="G50" s="4"/>
@@ -1985,7 +1985,7 @@
         <v>64</v>
       </c>
       <c r="C51" s="3"/>
-      <c r="D51" s="4"/>
+      <c r="D51" s="3"/>
       <c r="E51" s="4"/>
       <c r="F51" s="3"/>
       <c r="G51" s="4"/>
@@ -1999,7 +1999,7 @@
         <v>77</v>
       </c>
       <c r="C52" s="3"/>
-      <c r="D52" s="4"/>
+      <c r="D52" s="3"/>
       <c r="E52" s="4"/>
       <c r="F52" s="3"/>
       <c r="G52" s="4"/>
@@ -2013,7 +2013,7 @@
         <v>102</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="2"/>
+      <c r="D53" s="1"/>
       <c r="E53" s="2"/>
       <c r="F53" s="1"/>
       <c r="G53" s="2"/>
@@ -2027,7 +2027,7 @@
         <v>125</v>
       </c>
       <c r="C54" s="3"/>
-      <c r="D54" s="4"/>
+      <c r="D54" s="3"/>
       <c r="E54" s="4"/>
       <c r="F54" s="3"/>
       <c r="G54" s="4"/>
@@ -2041,7 +2041,7 @@
         <v>112</v>
       </c>
       <c r="C55" s="1"/>
-      <c r="D55" s="2"/>
+      <c r="D55" s="1"/>
       <c r="E55" s="2"/>
       <c r="F55" s="1"/>
       <c r="G55" s="2"/>
@@ -2055,7 +2055,7 @@
         <v>7</v>
       </c>
       <c r="C56" s="3"/>
-      <c r="D56" s="4"/>
+      <c r="D56" s="3"/>
       <c r="E56" s="4"/>
       <c r="F56" s="3"/>
       <c r="G56" s="4"/>
@@ -2069,7 +2069,7 @@
         <v>13</v>
       </c>
       <c r="C57" s="3"/>
-      <c r="D57" s="4"/>
+      <c r="D57" s="3"/>
       <c r="E57" s="4"/>
       <c r="F57" s="3"/>
       <c r="G57" s="4"/>
@@ -2083,7 +2083,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="1"/>
-      <c r="D58" s="2"/>
+      <c r="D58" s="1"/>
       <c r="E58" s="2"/>
       <c r="F58" s="1"/>
       <c r="G58" s="2"/>
@@ -2097,7 +2097,7 @@
         <v>7</v>
       </c>
       <c r="C59" s="3"/>
-      <c r="D59" s="4"/>
+      <c r="D59" s="3"/>
       <c r="E59" s="4"/>
       <c r="F59" s="3"/>
       <c r="G59" s="4"/>
@@ -2111,7 +2111,7 @@
         <v>79</v>
       </c>
       <c r="C60" s="1"/>
-      <c r="D60" s="2"/>
+      <c r="D60" s="1"/>
       <c r="E60" s="2"/>
       <c r="F60" s="1"/>
       <c r="G60" s="2"/>
@@ -2125,7 +2125,7 @@
         <v>37</v>
       </c>
       <c r="C61" s="1"/>
-      <c r="D61" s="2"/>
+      <c r="D61" s="1"/>
       <c r="E61" s="2"/>
       <c r="F61" s="1"/>
       <c r="G61" s="2"/>
@@ -2139,7 +2139,7 @@
         <v>105</v>
       </c>
       <c r="C62" s="3"/>
-      <c r="D62" s="4"/>
+      <c r="D62" s="3"/>
       <c r="E62" s="4"/>
       <c r="F62" s="3"/>
       <c r="G62" s="4"/>
@@ -2153,7 +2153,7 @@
         <v>105</v>
       </c>
       <c r="C63" s="1"/>
-      <c r="D63" s="2"/>
+      <c r="D63" s="1"/>
       <c r="E63" s="2"/>
       <c r="F63" s="1"/>
       <c r="G63" s="2"/>
@@ -2167,7 +2167,7 @@
         <v>97</v>
       </c>
       <c r="C64" s="3"/>
-      <c r="D64" s="4"/>
+      <c r="D64" s="3"/>
       <c r="E64" s="4"/>
       <c r="F64" s="3"/>
       <c r="G64" s="4"/>
@@ -2181,7 +2181,7 @@
         <v>105</v>
       </c>
       <c r="C65" s="3"/>
-      <c r="D65" s="4"/>
+      <c r="D65" s="3"/>
       <c r="E65" s="4"/>
       <c r="F65" s="3"/>
       <c r="G65" s="4"/>
@@ -2195,7 +2195,7 @@
         <v>43</v>
       </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="2"/>
+      <c r="D66" s="1"/>
       <c r="E66" s="2"/>
       <c r="F66" s="1"/>
       <c r="G66" s="2"/>
@@ -2209,7 +2209,7 @@
         <v>124</v>
       </c>
       <c r="C67" s="3"/>
-      <c r="D67" s="4"/>
+      <c r="D67" s="3"/>
       <c r="E67" s="4"/>
       <c r="F67" s="3"/>
       <c r="G67" s="4"/>
@@ -2223,7 +2223,7 @@
         <v>85</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="2"/>
+      <c r="D68" s="1"/>
       <c r="E68" s="2"/>
       <c r="F68" s="1"/>
       <c r="G68" s="2"/>
@@ -2237,7 +2237,7 @@
         <v>11</v>
       </c>
       <c r="C69" s="3"/>
-      <c r="D69" s="4"/>
+      <c r="D69" s="3"/>
       <c r="E69" s="4"/>
       <c r="F69" s="3"/>
       <c r="G69" s="4"/>
@@ -2251,7 +2251,7 @@
         <v>34</v>
       </c>
       <c r="C70" s="1"/>
-      <c r="D70" s="2"/>
+      <c r="D70" s="1"/>
       <c r="E70" s="2"/>
       <c r="F70" s="1"/>
       <c r="G70" s="2"/>
@@ -2265,7 +2265,7 @@
         <v>90</v>
       </c>
       <c r="C71" s="3"/>
-      <c r="D71" s="4"/>
+      <c r="D71" s="3"/>
       <c r="E71" s="4"/>
       <c r="F71" s="3"/>
       <c r="G71" s="4"/>
@@ -2279,7 +2279,7 @@
         <v>129</v>
       </c>
       <c r="C72" s="1"/>
-      <c r="D72" s="2"/>
+      <c r="D72" s="1"/>
       <c r="E72" s="2"/>
       <c r="F72" s="1"/>
       <c r="G72" s="2"/>
@@ -2293,7 +2293,7 @@
         <v>35</v>
       </c>
       <c r="C73" s="3"/>
-      <c r="D73" s="4"/>
+      <c r="D73" s="3"/>
       <c r="E73" s="4"/>
       <c r="F73" s="3"/>
       <c r="G73" s="4"/>
@@ -2307,7 +2307,7 @@
         <v>40</v>
       </c>
       <c r="C74" s="1"/>
-      <c r="D74" s="2"/>
+      <c r="D74" s="1"/>
       <c r="E74" s="2"/>
       <c r="F74" s="1"/>
       <c r="G74" s="2"/>
@@ -2321,7 +2321,7 @@
         <v>41</v>
       </c>
       <c r="C75" s="3"/>
-      <c r="D75" s="4"/>
+      <c r="D75" s="3"/>
       <c r="E75" s="4"/>
       <c r="F75" s="3"/>
       <c r="G75" s="4"/>
@@ -2335,7 +2335,7 @@
         <v>38</v>
       </c>
       <c r="C76" s="1"/>
-      <c r="D76" s="2"/>
+      <c r="D76" s="1"/>
       <c r="E76" s="2"/>
       <c r="F76" s="1"/>
       <c r="G76" s="2"/>
@@ -2349,7 +2349,7 @@
         <v>99</v>
       </c>
       <c r="C77" s="3"/>
-      <c r="D77" s="4"/>
+      <c r="D77" s="3"/>
       <c r="E77" s="4"/>
       <c r="F77" s="3"/>
       <c r="G77" s="4"/>
@@ -2363,7 +2363,7 @@
         <v>46</v>
       </c>
       <c r="C78" s="3"/>
-      <c r="D78" s="4"/>
+      <c r="D78" s="3"/>
       <c r="E78" s="4"/>
       <c r="F78" s="3"/>
       <c r="G78" s="4"/>
@@ -2377,7 +2377,7 @@
         <v>73</v>
       </c>
       <c r="C79" s="1"/>
-      <c r="D79" s="2"/>
+      <c r="D79" s="1"/>
       <c r="E79" s="2"/>
       <c r="F79" s="1"/>
       <c r="G79" s="2"/>
@@ -2391,7 +2391,7 @@
         <v>73</v>
       </c>
       <c r="C80" s="3"/>
-      <c r="D80" s="4"/>
+      <c r="D80" s="3"/>
       <c r="E80" s="4"/>
       <c r="F80" s="3"/>
       <c r="G80" s="4"/>
@@ -2405,7 +2405,7 @@
         <v>117</v>
       </c>
       <c r="C81" s="1"/>
-      <c r="D81" s="2"/>
+      <c r="D81" s="1"/>
       <c r="E81" s="2"/>
       <c r="F81" s="1"/>
       <c r="G81" s="2"/>
@@ -2419,7 +2419,7 @@
         <v>93</v>
       </c>
       <c r="C82" s="3"/>
-      <c r="D82" s="4"/>
+      <c r="D82" s="3"/>
       <c r="E82" s="4"/>
       <c r="F82" s="3"/>
       <c r="G82" s="4"/>
@@ -2433,7 +2433,7 @@
         <v>104</v>
       </c>
       <c r="C83" s="1"/>
-      <c r="D83" s="2"/>
+      <c r="D83" s="1"/>
       <c r="E83" s="2"/>
       <c r="F83" s="1"/>
       <c r="G83" s="2"/>
@@ -2447,7 +2447,7 @@
         <v>65</v>
       </c>
       <c r="C84" s="3"/>
-      <c r="D84" s="4"/>
+      <c r="D84" s="3"/>
       <c r="E84" s="4"/>
       <c r="F84" s="3"/>
       <c r="G84" s="4"/>
@@ -2461,7 +2461,7 @@
         <v>56</v>
       </c>
       <c r="C85" s="3"/>
-      <c r="D85" s="4"/>
+      <c r="D85" s="3"/>
       <c r="E85" s="4"/>
       <c r="F85" s="3"/>
       <c r="G85" s="4"/>
@@ -2475,7 +2475,7 @@
         <v>80</v>
       </c>
       <c r="C86" s="3"/>
-      <c r="D86" s="4"/>
+      <c r="D86" s="3"/>
       <c r="E86" s="4"/>
       <c r="F86" s="3"/>
       <c r="G86" s="4"/>
@@ -2489,7 +2489,7 @@
         <v>7</v>
       </c>
       <c r="C87" s="3"/>
-      <c r="D87" s="4"/>
+      <c r="D87" s="3"/>
       <c r="E87" s="4"/>
       <c r="F87" s="3"/>
       <c r="G87" s="4"/>
@@ -2503,7 +2503,7 @@
         <v>74</v>
       </c>
       <c r="C88" s="1"/>
-      <c r="D88" s="2"/>
+      <c r="D88" s="1"/>
       <c r="E88" s="2"/>
       <c r="F88" s="1"/>
       <c r="G88" s="2"/>
@@ -2517,7 +2517,7 @@
         <v>76</v>
       </c>
       <c r="C89" s="3"/>
-      <c r="D89" s="4"/>
+      <c r="D89" s="3"/>
       <c r="E89" s="4"/>
       <c r="F89" s="3"/>
       <c r="G89" s="4"/>
@@ -2531,7 +2531,7 @@
         <v>9</v>
       </c>
       <c r="C90" s="1"/>
-      <c r="D90" s="2"/>
+      <c r="D90" s="1"/>
       <c r="E90" s="2"/>
       <c r="F90" s="1"/>
       <c r="G90" s="2"/>
@@ -2545,7 +2545,7 @@
         <v>28</v>
       </c>
       <c r="C91" s="3"/>
-      <c r="D91" s="4"/>
+      <c r="D91" s="3"/>
       <c r="E91" s="4"/>
       <c r="F91" s="3"/>
       <c r="G91" s="4"/>
@@ -2559,7 +2559,7 @@
         <v>69</v>
       </c>
       <c r="C92" s="3"/>
-      <c r="D92" s="4"/>
+      <c r="D92" s="3"/>
       <c r="E92" s="4"/>
       <c r="F92" s="3"/>
       <c r="G92" s="4"/>
@@ -2573,7 +2573,7 @@
         <v>91</v>
       </c>
       <c r="C93" s="1"/>
-      <c r="D93" s="2"/>
+      <c r="D93" s="1"/>
       <c r="E93" s="2"/>
       <c r="F93" s="1"/>
       <c r="G93" s="2"/>
@@ -2587,7 +2587,7 @@
         <v>70</v>
       </c>
       <c r="C94" s="3"/>
-      <c r="D94" s="4"/>
+      <c r="D94" s="3"/>
       <c r="E94" s="4"/>
       <c r="F94" s="3"/>
       <c r="G94" s="4"/>
@@ -2601,7 +2601,7 @@
         <v>75</v>
       </c>
       <c r="C95" s="1"/>
-      <c r="D95" s="2"/>
+      <c r="D95" s="1"/>
       <c r="E95" s="2"/>
       <c r="F95" s="1"/>
       <c r="G95" s="2"/>
@@ -2615,7 +2615,7 @@
         <v>113</v>
       </c>
       <c r="C96" s="3"/>
-      <c r="D96" s="4"/>
+      <c r="D96" s="3"/>
       <c r="E96" s="4"/>
       <c r="F96" s="3"/>
       <c r="G96" s="4"/>
@@ -2629,7 +2629,7 @@
         <v>30</v>
       </c>
       <c r="C97" s="1"/>
-      <c r="D97" s="2"/>
+      <c r="D97" s="1"/>
       <c r="E97" s="2"/>
       <c r="F97" s="1"/>
       <c r="G97" s="2"/>
@@ -2643,7 +2643,7 @@
         <v>89</v>
       </c>
       <c r="C98" s="3"/>
-      <c r="D98" s="4"/>
+      <c r="D98" s="3"/>
       <c r="E98" s="4"/>
       <c r="F98" s="3"/>
       <c r="G98" s="4"/>
@@ -2657,7 +2657,7 @@
         <v>82</v>
       </c>
       <c r="C99" s="1"/>
-      <c r="D99" s="2"/>
+      <c r="D99" s="1"/>
       <c r="E99" s="2"/>
       <c r="F99" s="1"/>
       <c r="G99" s="2"/>
@@ -2671,7 +2671,7 @@
         <v>115</v>
       </c>
       <c r="C100" s="3"/>
-      <c r="D100" s="4"/>
+      <c r="D100" s="3"/>
       <c r="E100" s="4"/>
       <c r="F100" s="3"/>
       <c r="G100" s="4"/>
@@ -2685,7 +2685,7 @@
         <v>101</v>
       </c>
       <c r="C101" s="1"/>
-      <c r="D101" s="2"/>
+      <c r="D101" s="1"/>
       <c r="E101" s="2"/>
       <c r="F101" s="1"/>
       <c r="G101" s="2"/>
@@ -2699,7 +2699,7 @@
         <v>42</v>
       </c>
       <c r="C102" s="3"/>
-      <c r="D102" s="4"/>
+      <c r="D102" s="3"/>
       <c r="E102" s="4"/>
       <c r="F102" s="3"/>
       <c r="G102" s="4"/>
@@ -2713,7 +2713,7 @@
         <v>63</v>
       </c>
       <c r="C103" s="1"/>
-      <c r="D103" s="2"/>
+      <c r="D103" s="1"/>
       <c r="E103" s="2"/>
       <c r="F103" s="1"/>
       <c r="G103" s="2"/>
@@ -2727,7 +2727,7 @@
         <v>88</v>
       </c>
       <c r="C104" s="1"/>
-      <c r="D104" s="2"/>
+      <c r="D104" s="1"/>
       <c r="E104" s="2"/>
       <c r="F104" s="1"/>
       <c r="G104" s="2"/>
@@ -2741,7 +2741,7 @@
         <v>110</v>
       </c>
       <c r="C105" s="3"/>
-      <c r="D105" s="4"/>
+      <c r="D105" s="3"/>
       <c r="E105" s="4"/>
       <c r="F105" s="3"/>
       <c r="G105" s="4"/>
@@ -2755,7 +2755,7 @@
         <v>26</v>
       </c>
       <c r="C106" s="1"/>
-      <c r="D106" s="2"/>
+      <c r="D106" s="1"/>
       <c r="E106" s="2"/>
       <c r="F106" s="1"/>
       <c r="G106" s="2"/>
@@ -2769,7 +2769,7 @@
         <v>108</v>
       </c>
       <c r="C107" s="1"/>
-      <c r="D107" s="2"/>
+      <c r="D107" s="1"/>
       <c r="E107" s="2"/>
       <c r="F107" s="1"/>
       <c r="G107" s="2"/>
@@ -2783,7 +2783,7 @@
         <v>58</v>
       </c>
       <c r="C108" s="3"/>
-      <c r="D108" s="4"/>
+      <c r="D108" s="3"/>
       <c r="E108" s="4"/>
       <c r="F108" s="3"/>
       <c r="G108" s="4"/>
@@ -2797,7 +2797,7 @@
         <v>7</v>
       </c>
       <c r="C109" s="1"/>
-      <c r="D109" s="2"/>
+      <c r="D109" s="1"/>
       <c r="E109" s="2"/>
       <c r="F109" s="1"/>
       <c r="G109" s="2"/>
@@ -2811,7 +2811,7 @@
         <v>122</v>
       </c>
       <c r="C110" s="3"/>
-      <c r="D110" s="4"/>
+      <c r="D110" s="3"/>
       <c r="E110" s="4"/>
       <c r="F110" s="3"/>
       <c r="G110" s="4"/>
@@ -2825,7 +2825,7 @@
         <v>68</v>
       </c>
       <c r="C111" s="3"/>
-      <c r="D111" s="4"/>
+      <c r="D111" s="3"/>
       <c r="E111" s="4"/>
       <c r="F111" s="3"/>
       <c r="G111" s="4"/>
@@ -2839,7 +2839,7 @@
         <v>51</v>
       </c>
       <c r="C112" s="1"/>
-      <c r="D112" s="2"/>
+      <c r="D112" s="1"/>
       <c r="E112" s="2"/>
       <c r="F112" s="1"/>
       <c r="G112" s="2"/>
@@ -2853,7 +2853,7 @@
         <v>135</v>
       </c>
       <c r="C113" s="3"/>
-      <c r="D113" s="4"/>
+      <c r="D113" s="3"/>
       <c r="E113" s="4"/>
       <c r="F113" s="3"/>
       <c r="G113" s="4"/>
@@ -2867,7 +2867,7 @@
         <v>55</v>
       </c>
       <c r="C114" s="1"/>
-      <c r="D114" s="2"/>
+      <c r="D114" s="1"/>
       <c r="E114" s="2"/>
       <c r="F114" s="1"/>
       <c r="G114" s="2"/>
@@ -2881,7 +2881,7 @@
         <v>100</v>
       </c>
       <c r="C115" s="1"/>
-      <c r="D115" s="2"/>
+      <c r="D115" s="1"/>
       <c r="E115" s="2"/>
       <c r="F115" s="1"/>
       <c r="G115" s="2"/>
@@ -2895,7 +2895,7 @@
         <v>119</v>
       </c>
       <c r="C116" s="1"/>
-      <c r="D116" s="2"/>
+      <c r="D116" s="1"/>
       <c r="E116" s="2"/>
       <c r="F116" s="1"/>
       <c r="G116" s="2"/>
@@ -2909,7 +2909,7 @@
         <v>121</v>
       </c>
       <c r="C117" s="7"/>
-      <c r="D117" s="8"/>
+      <c r="D117" s="7"/>
       <c r="E117" s="8"/>
       <c r="F117" s="7"/>
       <c r="G117" s="8"/>
@@ -2925,10 +2925,10 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>